<commit_message>
feat: add faceted cognitive lifespan charts answering SQ2
</commit_message>
<xml_diff>
--- a/examples/single_agent/analysis/sq1_metrics_rules.xlsx
+++ b/examples/single_agent/analysis/sq1_metrics_rules.xlsx
@@ -85,7 +85,7 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Y3</t>
+    <t>Y4</t>
   </si>
   <si>
     <t>deepseek_r1_1_5b</t>
@@ -1122,22 +1122,22 @@
     </row>
     <row r="11" spans="1:21">
       <c r="A11">
-        <v>298</v>
+        <v>393</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>298</v>
+        <v>391</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1146,10 +1146,10 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>51.7</v>
+        <v>45</v>
       </c>
       <c r="J11">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1158,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>44</v>
+        <v>45.3</v>
       </c>
       <c r="N11" t="s">
         <v>23</v>
@@ -1170,19 +1170,19 @@
         <v>28</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11">
-        <v>51.7</v>
+        <v>45</v>
       </c>
       <c r="U11">
-        <v>44</v>
+        <v>45.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: complete SQ1 and SQ2 analysis packages and final synthesis
</commit_message>
<xml_diff>
--- a/examples/single_agent/analysis/sq1_metrics_rules.xlsx
+++ b/examples/single_agent/analysis/sq1_metrics_rules.xlsx
@@ -85,7 +85,7 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Y4</t>
+    <t>Y7</t>
   </si>
   <si>
     <t>deepseek_r1_1_5b</t>
@@ -1122,22 +1122,22 @@
     </row>
     <row r="11" spans="1:21">
       <c r="A11">
-        <v>393</v>
+        <v>687</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C11">
-        <v>391</v>
+        <v>661</v>
       </c>
       <c r="D11">
-        <v>0.5</v>
+        <v>3.8</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1146,10 +1146,10 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>45</v>
+        <v>33.9</v>
       </c>
       <c r="J11">
-        <v>177</v>
+        <v>233</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1158,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>45.3</v>
+        <v>31.18</v>
       </c>
       <c r="N11" t="s">
         <v>23</v>
@@ -1170,19 +1170,19 @@
         <v>28</v>
       </c>
       <c r="Q11">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="R11">
-        <v>0.5</v>
+        <v>3.8</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11">
-        <v>45</v>
+        <v>33.9</v>
       </c>
       <c r="U11">
-        <v>45.3</v>
+        <v>31.18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>